<commit_message>
update excel file of student
</commit_message>
<xml_diff>
--- a/docker/files/RandomStudent/Education system.xlsx
+++ b/docker/files/RandomStudent/Education system.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge\repository\basedatosII\docker\files\RandomStudent\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santosj.MIXCO\repository\basedatosII\docker\files\RandomStudent\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12885" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Pensum" sheetId="1" r:id="rId1"/>
@@ -757,7 +757,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -774,7 +774,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1038,13 +1038,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="B2:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.85546875" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
@@ -3206,7 +3206,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
@@ -3454,7 +3454,7 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.28515625" customWidth="1"/>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
@@ -3854,11 +3854,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
@@ -4097,7 +4097,7 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>